<commit_message>
renamed test data files, grouped in their own folders
</commit_message>
<xml_diff>
--- a/data/exam_1_scores.xlsx
+++ b/data/exam_1_scores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7ABF321-5ACA-430F-8C7D-3A6C74725700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59852AE0-CAD7-41E8-B98E-709B5476DF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>